<commit_message>
Added Graph to Version 2
</commit_message>
<xml_diff>
--- a/Version 2 Liang–Barsky algorithm By Abrar.xlsx
+++ b/Version 2 Liang–Barsky algorithm By Abrar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\Liang_Barsky_algorithm_Computer_Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB17094-1DD2-450C-9721-4F6388D17841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B7E82-1C1A-4FF8-934A-A114C8DE1DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ENTER Minimum Point of Window</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Pmax</t>
   </si>
   <si>
-    <t>LINE 1</t>
-  </si>
-  <si>
     <t>P0</t>
   </si>
   <si>
@@ -115,12 +112,6 @@
   </si>
   <si>
     <t>ENTER FIRST Point</t>
-  </si>
-  <si>
-    <t>1,</t>
-  </si>
-  <si>
-    <t>LINE2</t>
   </si>
   <si>
     <t>te = max(0, ALL PE)</t>
@@ -189,13 +180,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -213,6 +204,1145 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graph of Window And Line</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$2:$Y$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Z$2:$Z$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BF2-4F63-B5D5-D888985D73E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LIne</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$K$7,Sheet1!$K$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$L$7,Sheet1!$L$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9BF2-4F63-B5D5-D888985D73E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="401177359"/>
+        <c:axId val="401166127"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="401177359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401166127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401166127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401177359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF0D9C96-79AC-4702-B34D-BDCFA07BBF54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,15 +1608,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V27"/>
+  <dimension ref="B1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:26" x14ac:dyDescent="0.3">
       <c r="K1" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,217 +1624,229 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E2" s="4" t="s">
+    <row r="2" spans="3:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="3:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="Y2">
+        <f>K2</f>
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <f>L2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="3:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="P3" t="s">
         <v>6</v>
       </c>
-      <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3">
-        <v>4</v>
-      </c>
-      <c r="U3">
-        <v>8</v>
-      </c>
-      <c r="V3">
+      <c r="Y3">
+        <f>K3</f>
+        <v>6</v>
+      </c>
+      <c r="Z3">
+        <f>L2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="Y4">
+        <f>K3</f>
+        <v>6</v>
+      </c>
+      <c r="Z4">
+        <f>L3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="Y5">
+        <f>K2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="P4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>7</v>
-      </c>
-      <c r="V4">
+      <c r="Z5">
+        <f>L3</f>
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="F7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="Y6">
+        <f>K2</f>
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <f>L2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.3">
       <c r="I9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9">
         <f>K8-K7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I10" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="J10" s="3"/>
       <c r="L10">
         <f>L8-L7</f>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.3">
       <c r="I11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11">
         <f>(K2-K7)/K9</f>
-        <v>0.33333333333333331</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="M11" t="str">
         <f>IF(K12&gt;0,"PL","PE")</f>
         <v>PE</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="6"/>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="I12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5"/>
       <c r="K12">
         <f>-K9</f>
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.3">
       <c r="I13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13">
         <f>(K3-K7)/K9</f>
-        <v>0.88888888888888884</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="M13" t="str">
         <f>IF(K14&gt;0,"PL","PE")</f>
         <v>PL</v>
       </c>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="6"/>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="I14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="5"/>
       <c r="K14">
         <f>K9</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.3">
       <c r="I15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" s="3"/>
       <c r="L15">
         <f>(L2-L7)/L10</f>
-        <v>0.7142857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="M15" t="str">
         <f>IF(L16&gt;0,"PL","PE")</f>
         <v>PL</v>
       </c>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="6"/>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="I16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="5"/>
       <c r="L16">
         <f>-L10</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17" s="3"/>
       <c r="L17">
         <f>(L3-L7)/L10</f>
-        <v>0.2857142857142857</v>
+        <v>-1</v>
       </c>
       <c r="M17" t="str">
         <f>IF(L18&gt;0,"PL","PE")</f>
@@ -712,13 +1854,13 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="6"/>
+      <c r="I18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="5"/>
       <c r="L18">
         <f>L10</f>
-        <v>-7</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
@@ -726,23 +1868,23 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="6"/>
+      <c r="I20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="5"/>
       <c r="K20">
         <f>IF(K12&lt;0, IF(L18&lt;0, MAX(K11,L17,0),MAX(K11,L15,0)),IF(L18&lt;0, MAX(K13,L17,0),MAX(K13,L15,0)))</f>
-        <v>0.33333333333333331</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I21" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21">
         <f>IF(K13&gt;0, IF(L16&gt;0, MIN(K13,L15,1),MIN(K13,L17,1)), IF(L16&gt;0, MIN(K11,L15,1),MIN(K11,L17,1)))</f>
-        <v>0.7142857142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
@@ -750,59 +1892,70 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24">
-        <f>IF(K7&lt;K8,K7+K20*(K9),"NOT POSSIBLE")</f>
-        <v>6</v>
+        <f>IF(K20&lt;K21,K7+K20*(K9),"LINE OUTSIDE")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25">
-        <f>IF(K7&lt;K8,L7+K20*L10,"NOT POSSIBLE")</f>
-        <v>7.666666666666667</v>
+        <f>IF(K20&lt;K21,L7+K20*L10,"LINE OUTSIDE")</f>
+        <v>3.7142857142857144</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26">
-        <f>IF(K7&lt;K8,K7+K21*(K9),"NOT POSSIBLE")</f>
-        <v>9.4285714285714288</v>
+        <f>IF(K20&lt;K21,K7+K21*(K9),"LINE OUTSIDE")</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27">
-        <f>IF(K7&lt;K8,L7+K21*L10,"NOT POSSIBLE")</f>
-        <v>5</v>
+        <f>IF(K20&lt;K21,L7+K21*L10,"LINE OUTSIDE")</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="B26:D26"/>
@@ -819,19 +1972,9 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Images for Screenshot
</commit_message>
<xml_diff>
--- a/Version 2 Liang–Barsky algorithm By Abrar.xlsx
+++ b/Version 2 Liang–Barsky algorithm By Abrar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\Liang_Barsky_algorithm_Computer_Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B7E82-1C1A-4FF8-934A-A114C8DE1DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E8FA9-32F0-43A5-BB4C-E346558F536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,15 +99,6 @@
     <t>CARTESIAN CO ORDINATE</t>
   </si>
   <si>
-    <t>P1y(t) = P0y+(P1y-P0y)*te</t>
-  </si>
-  <si>
-    <t>Px(te) = P0x+(P1x-P0x)*tl</t>
-  </si>
-  <si>
-    <t>P1y(t) = P0y+(P1y-P0y)*tl</t>
-  </si>
-  <si>
     <t>ENTER SECOND Point</t>
   </si>
   <si>
@@ -118,6 +109,15 @@
   </si>
   <si>
     <t>tl = min(1, ALL PL)</t>
+  </si>
+  <si>
+    <t>P1y(te) = P0y+(P1y-P0y)*te</t>
+  </si>
+  <si>
+    <t>Px(tl) = P0x+(P1x-P0x)*tl</t>
+  </si>
+  <si>
+    <t>P1y(tl) = P0y+(P1y-P0y)*tl</t>
   </si>
 </sst>
 </file>
@@ -177,6 +177,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -184,9 +187,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -528,7 +528,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -582,8 +582,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1608,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Z27"/>
+  <dimension ref="C1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,16 +1626,16 @@
       </c>
     </row>
     <row r="2" spans="3:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="4"/>
       <c r="K2">
         <v>2</v>
       </c>
@@ -1651,16 +1652,16 @@
       </c>
     </row>
     <row r="3" spans="3:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="4"/>
       <c r="K3">
         <v>6</v>
       </c>
@@ -1697,13 +1698,13 @@
       </c>
     </row>
     <row r="6" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="Y6">
         <f>K2</f>
         <v>2</v>
@@ -1714,32 +1715,32 @@
       </c>
     </row>
     <row r="7" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="4"/>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3" t="s">
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="4"/>
       <c r="K8">
         <v>8</v>
       </c>
@@ -1748,30 +1749,30 @@
       </c>
     </row>
     <row r="9" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
       <c r="K9">
         <f>K8-K7</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="4"/>
       <c r="L10">
         <f>L8-L7</f>
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="4"/>
       <c r="K11">
         <f>(K2-K7)/K9</f>
         <v>0.14285714285714285</v>
@@ -1782,20 +1783,20 @@
       </c>
     </row>
     <row r="12" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="6"/>
       <c r="K12">
         <f>-K9</f>
         <v>-7</v>
       </c>
     </row>
     <row r="13" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="3"/>
+      <c r="J13" s="4"/>
       <c r="K13">
         <f>(K3-K7)/K9</f>
         <v>0.7142857142857143</v>
@@ -1806,172 +1807,172 @@
       </c>
     </row>
     <row r="14" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="6"/>
       <c r="K14">
         <f>K9</f>
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="4"/>
       <c r="L15">
         <f>(L2-L7)/L10</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="M15" t="str">
         <f>IF(L16&gt;0,"PL","PE")</f>
-        <v>PL</v>
+        <v>PE</v>
       </c>
     </row>
     <row r="16" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="6"/>
       <c r="L16">
         <f>-L10</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I17" s="3" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="I17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="J17" s="4"/>
       <c r="L17">
         <f>(L3-L7)/L10</f>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M17" t="str">
         <f>IF(L18&gt;0,"PL","PE")</f>
-        <v>PE</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I18" s="5" t="s">
+        <v>PL</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="I18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18" s="6"/>
       <c r="L18">
         <f>L10</f>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="I20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="6"/>
       <c r="K20">
         <f>IF(K12&lt;0, IF(L18&lt;0, MAX(K11,L17,0),MAX(K11,L15,0)),IF(L18&lt;0, MAX(K13,L17,0),MAX(K13,L15,0)))</f>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21" s="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="I21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="4"/>
       <c r="K21">
         <f>IF(K13&gt;0, IF(L16&gt;0, MIN(K13,L15,1),MIN(K13,L17,1)), IF(L16&gt;0, MIN(K11,L15,1),MIN(K11,L17,1)))</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.3">
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" t="str">
         <f>IF(K20&lt;K21,K7+K20*(K9),"LINE OUTSIDE")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25">
+        <v>LINE OUTSIDE</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" t="str">
         <f>IF(K20&lt;K21,L7+K20*L10,"LINE OUTSIDE")</f>
-        <v>3.7142857142857144</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26">
+        <v>LINE OUTSIDE</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" t="str">
         <f>IF(K20&lt;K21,K7+K21*(K9),"LINE OUTSIDE")</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27">
+        <v>LINE OUTSIDE</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" t="str">
         <f>IF(K20&lt;K21,L7+K21*L10,"LINE OUTSIDE")</f>
-        <v>3</v>
+        <v>LINE OUTSIDE</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>